<commit_message>
Version 2025 by Alberto
</commit_message>
<xml_diff>
--- a/data/spetses_school_codebook.xlsx
+++ b/data/spetses_school_codebook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28005"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ecdc365-my.sharepoint.com/personal/pawel_stefanoff_ecdc_europa_eu/Documents/Documents/MediPIET/Modules/2024/09-IntroCourse/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateourdiales_albert\Documents\GitHub\IntroCourse_inCop\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="11_DF23370A8E1D283A0172E3E9E763439A928E986D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF547CE4-7465-4000-B89B-9A4756508999}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87DF2716-8802-42F0-83CC-466DF1A29B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="97">
   <si>
     <t>Variable</t>
   </si>
@@ -203,42 +203,6 @@
     <t>Quantity of eggplant dip eaten</t>
   </si>
   <si>
-    <t>moussaka</t>
-  </si>
-  <si>
-    <t>Ate vegetetarian moussaka</t>
-  </si>
-  <si>
-    <t>moussakaD</t>
-  </si>
-  <si>
-    <t>Quantity of moussaka eaten</t>
-  </si>
-  <si>
-    <t>orzo</t>
-  </si>
-  <si>
-    <t>Ate creamy chicken orzo</t>
-  </si>
-  <si>
-    <t>orzoD</t>
-  </si>
-  <si>
-    <t>Quantity of orzo eaten</t>
-  </si>
-  <si>
-    <t>greeksal</t>
-  </si>
-  <si>
-    <t>Ate Greek salad</t>
-  </si>
-  <si>
-    <t>greeksalD</t>
-  </si>
-  <si>
-    <t>Quantity of Greek salad eaten</t>
-  </si>
-  <si>
     <t>bread</t>
   </si>
   <si>
@@ -318,13 +282,58 @@
   </si>
   <si>
     <t>date with day, month and year</t>
+  </si>
+  <si>
+    <t>ill</t>
+  </si>
+  <si>
+    <t>felt ill after the school party</t>
+  </si>
+  <si>
+    <t>0 = did not feel ill after the school party; 1 = felt ill after the school party</t>
+  </si>
+  <si>
+    <t>pasta</t>
+  </si>
+  <si>
+    <t>ate pasta salad with pesto</t>
+  </si>
+  <si>
+    <t>pastaD</t>
+  </si>
+  <si>
+    <t>quantity of pasta salad woth pesto eaten</t>
+  </si>
+  <si>
+    <t>veal</t>
+  </si>
+  <si>
+    <t>ate roasted veal</t>
+  </si>
+  <si>
+    <t>vealD</t>
+  </si>
+  <si>
+    <t>quantity of roasted veal eaten</t>
+  </si>
+  <si>
+    <t>tomsal</t>
+  </si>
+  <si>
+    <t>Ate tomato with olive oil salad</t>
+  </si>
+  <si>
+    <t>Quantity of tomato with olive oil salad eaten</t>
+  </si>
+  <si>
+    <t>tomsalD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -341,12 +350,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -361,18 +376,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -388,9 +404,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -428,7 +444,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -534,7 +550,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -676,7 +692,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -684,469 +700,481 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31:C32"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A6" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.42578125" customWidth="1"/>
-    <col min="3" max="3" width="83.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.3984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="83.73046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.73046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>24</v>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>26</v>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>28</v>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>30</v>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>32</v>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>34</v>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B16" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A17" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A18" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B18" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A19" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B19" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A20" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A21" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A22" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A23" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A24" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A25" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A26" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A27" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A28" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A29" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A30" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B30" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C30" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A31" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B31" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C31" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A32" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B32" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C32" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A33" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B33" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C33" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
-      <c r="A27" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A34" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B34" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C34" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
-      <c r="A28" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A35" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B35" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C35" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
-      <c r="A29" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A36" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B36" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C36" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
-      <c r="A30" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A37" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B37" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C37" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
-      <c r="A31" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A38" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B38" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C38" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
-      <c r="A32" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A39" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B39" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C39" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
-      <c r="A33" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A40" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B40" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C40" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
-      <c r="A34" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A41" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B41" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C41" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A42" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B42" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C35" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" t="s">
+      <c r="C42" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="B36" t="s">
-        <v>82</v>
-      </c>
-      <c r="C36" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" t="s">
-        <v>83</v>
-      </c>
-      <c r="B37" t="s">
-        <v>84</v>
-      </c>
-      <c r="C37" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" t="s">
-        <v>85</v>
-      </c>
-      <c r="B38" t="s">
-        <v>86</v>
-      </c>
-      <c r="C38" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" t="s">
-        <v>87</v>
-      </c>
-      <c r="B39" t="s">
-        <v>88</v>
-      </c>
-      <c r="C39" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" t="s">
-        <v>89</v>
-      </c>
-      <c r="B40" t="s">
-        <v>90</v>
-      </c>
-      <c r="C40" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" t="s">
-        <v>91</v>
-      </c>
-      <c r="B41" t="s">
-        <v>92</v>
-      </c>
-      <c r="C41" t="s">
-        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1159,6 +1187,129 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="14c281f0-fdb2-43d6-8bd5-8268950107ba" ContentTypeId="0x010100EE95EE7DB3A482488E68FA4A7091999F" PreviousValue="false" LastSyncTimeStamp="2023-05-23T07:48:25.837Z"/>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <b489bfe21c7249aba6a1ae186fa4e51c xmlns="fe73b3f6-a427-4a99-886e-da32c6de835d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Draft</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">bed60e9a-f1b8-4691-a7e2-534f78067ff3</TermId>
+        </TermInfo>
+      </Terms>
+    </b489bfe21c7249aba6a1ae186fa4e51c>
+    <ECMX_SUMMARY xmlns="4240f11c-4df2-4a37-9be1-bdf0d4dfc218" xsi:nil="true"/>
+    <ECMX_ADDITIONALINFO xmlns="4240f11c-4df2-4a37-9be1-bdf0d4dfc218" xsi:nil="true"/>
+    <ECMX_OWNER xmlns="fe73b3f6-a427-4a99-886e-da32c6de835d">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </ECMX_OWNER>
+    <kf1264ba1b22407abef15b09c01e8cf0 xmlns="fe73b3f6-a427-4a99-886e-da32c6de835d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </kf1264ba1b22407abef15b09c01e8cf0>
+    <TaxKeywordTaxHTField xmlns="236fb19c-531c-4906-93ff-6da175312317">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <o13d78bceb4b4178ab3c456bf4db706a xmlns="fe73b3f6-a427-4a99-886e-da32c6de835d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </o13d78bceb4b4178ab3c456bf4db706a>
+    <ECMX_PUBLISHDATE xmlns="4240f11c-4df2-4a37-9be1-bdf0d4dfc218" xsi:nil="true"/>
+    <ECMX_BUSINESSID xmlns="4240f11c-4df2-4a37-9be1-bdf0d4dfc218" xsi:nil="true"/>
+    <c67668d6730c4bc2a26c654fc875ab99 xmlns="fe73b3f6-a427-4a99-886e-da32c6de835d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </c67668d6730c4bc2a26c654fc875ab99>
+    <TaxCatchAll xmlns="fe73b3f6-a427-4a99-886e-da32c6de835d">
+      <Value>2</Value>
+      <Value>1</Value>
+    </TaxCatchAll>
+    <na274824997947589a1bfdfb0b645b50 xmlns="fe73b3f6-a427-4a99-886e-da32c6de835d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </na274824997947589a1bfdfb0b645b50>
+    <ECMX_OPERATIONALID xmlns="4240f11c-4df2-4a37-9be1-bdf0d4dfc218" xsi:nil="true"/>
+    <cbaf9fdaaf87475a8d0ae10d3e79318e xmlns="fe73b3f6-a427-4a99-886e-da32c6de835d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Active</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">50127695-0d4f-4ac1-ab93-ebc716c3e584</TermId>
+        </TermInfo>
+      </Terms>
+    </cbaf9fdaaf87475a8d0ae10d3e79318e>
+    <_dlc_DocId xmlns="236fb19c-531c-4906-93ff-6da175312317">ObSiom24-1338803985-42</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="236fb19c-531c-4906-93ff-6da175312317">
+      <Url>https://ecdc365.sharepoint.com/teams/econ_obsiom24/_layouts/15/DocIdRedir.aspx?ID=ObSiom24-1338803985-42</Url>
+      <Description>ObSiom24-1338803985-42</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Standard Document" ma:contentTypeID="0x010100EE95EE7DB3A482488E68FA4A7091999F003CCD4A4BFBBE2C43A47767A144F9EFED" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6a2c1177e0b69ea6cfd36c2bda2b2415">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4240f11c-4df2-4a37-9be1-bdf0d4dfc218" xmlns:ns3="fe73b3f6-a427-4a99-886e-da32c6de835d" xmlns:ns4="236fb19c-531c-4906-93ff-6da175312317" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="488faa49e5aa9ebf8092283bde2cbd00" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="4240f11c-4df2-4a37-9be1-bdf0d4dfc218"/>
@@ -1451,147 +1602,60 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <b489bfe21c7249aba6a1ae186fa4e51c xmlns="fe73b3f6-a427-4a99-886e-da32c6de835d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Draft</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">bed60e9a-f1b8-4691-a7e2-534f78067ff3</TermId>
-        </TermInfo>
-      </Terms>
-    </b489bfe21c7249aba6a1ae186fa4e51c>
-    <ECMX_SUMMARY xmlns="4240f11c-4df2-4a37-9be1-bdf0d4dfc218" xsi:nil="true"/>
-    <ECMX_ADDITIONALINFO xmlns="4240f11c-4df2-4a37-9be1-bdf0d4dfc218" xsi:nil="true"/>
-    <ECMX_OWNER xmlns="fe73b3f6-a427-4a99-886e-da32c6de835d">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </ECMX_OWNER>
-    <kf1264ba1b22407abef15b09c01e8cf0 xmlns="fe73b3f6-a427-4a99-886e-da32c6de835d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </kf1264ba1b22407abef15b09c01e8cf0>
-    <TaxKeywordTaxHTField xmlns="236fb19c-531c-4906-93ff-6da175312317">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-    <o13d78bceb4b4178ab3c456bf4db706a xmlns="fe73b3f6-a427-4a99-886e-da32c6de835d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </o13d78bceb4b4178ab3c456bf4db706a>
-    <ECMX_PUBLISHDATE xmlns="4240f11c-4df2-4a37-9be1-bdf0d4dfc218" xsi:nil="true"/>
-    <ECMX_BUSINESSID xmlns="4240f11c-4df2-4a37-9be1-bdf0d4dfc218" xsi:nil="true"/>
-    <c67668d6730c4bc2a26c654fc875ab99 xmlns="fe73b3f6-a427-4a99-886e-da32c6de835d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </c67668d6730c4bc2a26c654fc875ab99>
-    <TaxCatchAll xmlns="fe73b3f6-a427-4a99-886e-da32c6de835d">
-      <Value>2</Value>
-      <Value>1</Value>
-    </TaxCatchAll>
-    <na274824997947589a1bfdfb0b645b50 xmlns="fe73b3f6-a427-4a99-886e-da32c6de835d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </na274824997947589a1bfdfb0b645b50>
-    <ECMX_OPERATIONALID xmlns="4240f11c-4df2-4a37-9be1-bdf0d4dfc218" xsi:nil="true"/>
-    <cbaf9fdaaf87475a8d0ae10d3e79318e xmlns="fe73b3f6-a427-4a99-886e-da32c6de835d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Active</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">50127695-0d4f-4ac1-ab93-ebc716c3e584</TermId>
-        </TermInfo>
-      </Terms>
-    </cbaf9fdaaf87475a8d0ae10d3e79318e>
-    <_dlc_DocId xmlns="236fb19c-531c-4906-93ff-6da175312317">ObSiom24-1338803985-42</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="236fb19c-531c-4906-93ff-6da175312317">
-      <Url>https://ecdc365.sharepoint.com/teams/econ_obsiom24/_layouts/15/DocIdRedir.aspx?ID=ObSiom24-1338803985-42</Url>
-      <Description>ObSiom24-1338803985-42</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="14c281f0-fdb2-43d6-8bd5-8268950107ba" ContentTypeId="0x010100EE95EE7DB3A482488E68FA4A7091999F" PreviousValue="false" LastSyncTimeStamp="2023-05-23T07:48:25.837Z"/>
-</file>
-
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB02B692-8DF8-45D5-AEB4-4C6C7A1C7E25}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC65E79F-B444-4CC5-A2C8-A0F1031C1C6B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1ACA882-8AB7-42A5-BB2A-748205E525B0}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C15BAB8-A620-4B16-9847-2341B3703619}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB1BA963-5AE0-44EF-8179-FF832DB83127}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB1BA963-5AE0-44EF-8179-FF832DB83127}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C15BAB8-A620-4B16-9847-2341B3703619}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1ACA882-8AB7-42A5-BB2A-748205E525B0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="fe73b3f6-a427-4a99-886e-da32c6de835d"/>
+    <ds:schemaRef ds:uri="4240f11c-4df2-4a37-9be1-bdf0d4dfc218"/>
+    <ds:schemaRef ds:uri="236fb19c-531c-4906-93ff-6da175312317"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC65E79F-B444-4CC5-A2C8-A0F1031C1C6B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB02B692-8DF8-45D5-AEB4-4C6C7A1C7E25}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="4240f11c-4df2-4a37-9be1-bdf0d4dfc218"/>
+    <ds:schemaRef ds:uri="fe73b3f6-a427-4a99-886e-da32c6de835d"/>
+    <ds:schemaRef ds:uri="236fb19c-531c-4906-93ff-6da175312317"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>